<commit_message>
Working with new format
</commit_message>
<xml_diff>
--- a/client/public/VC_Capability_Master.xlsx
+++ b/client/public/VC_Capability_Master.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Project\Value chain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Project\ValueChainSite\ValueChainIntelligence\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E235A0-3259-43C4-8864-DC4F28C5428A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E34AB3E-B0B3-4B9D-AB3F-6F1849AFCCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{BD5DD5E2-53C9-C848-BED8-5645BBCDEF26}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="439">
   <si>
     <t>Capability Name</t>
   </si>
@@ -1280,9 +1280,6 @@
     <t>Media Production</t>
   </si>
   <si>
-    <t>Shipping (Ocean Carrier - VOCC)</t>
-  </si>
-  <si>
     <t>Logistics (3PL/4PL/Forwarders - NVOCC)</t>
   </si>
   <si>
@@ -1319,9 +1316,6 @@
     <t>Annual Revenues (US$)</t>
   </si>
   <si>
-    <t>Strategic Focus</t>
-  </si>
-  <si>
     <t>Single Country</t>
   </si>
   <si>
@@ -1331,9 +1325,6 @@
     <t>100,000-1M</t>
   </si>
   <si>
-    <t>Original Growth</t>
-  </si>
-  <si>
     <t>Regional</t>
   </si>
   <si>
@@ -1343,9 +1334,6 @@
     <t>1M-100M</t>
   </si>
   <si>
-    <t>Inorganic Growth (M&amp;A)</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
@@ -1355,28 +1343,22 @@
     <t>100M-1B</t>
   </si>
   <si>
-    <t>Cost Optimization</t>
-  </si>
-  <si>
     <t>1B &amp; More</t>
   </si>
   <si>
-    <t>Digital Transformation</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>This is a temporary description and need to be changed later. Make sure to change it during production deployment</t>
   </si>
   <si>
-    <t>Shipping (Ocean Carrier - VOCC), Logistics (3PL/4PL/Forwarders - NVOCC)</t>
-  </si>
-  <si>
-    <t>Shipping (Ocean Carrier - VOCC), Logistics (3PL/4PL/Forwarders - NVOCC), Retail (General Merchandise)</t>
-  </si>
-  <si>
     <t>Business Type</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Shipping, Logistics (3PL/4PL/Forwarders - NVOCC)</t>
+  </si>
+  <si>
+    <t>Shipping, Logistics (3PL/4PL/Forwarders - NVOCC), Retail (General Merchandise)</t>
   </si>
 </sst>
 </file>
@@ -1842,10 +1824,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1854,163 +1836,123 @@
     <col min="2" max="2" width="16.4140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.4140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>422</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>423</v>
       </c>
-      <c r="D1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="D2" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>214</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>255</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>256</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
-        <v>277</v>
-      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="10" t="s">
-        <v>298</v>
-      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="10" t="s">
-        <v>319</v>
-      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="10" t="s">
-        <v>340</v>
-      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="10" t="s">
-        <v>361</v>
-      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="10" t="s">
-        <v>382</v>
-      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="10" t="s">
-        <v>411</v>
-      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2022,7 +1964,7 @@
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2049,7 +1991,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>174</v>
@@ -2058,12 +2000,12 @@
         <v>175</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>176</v>
@@ -2072,12 +2014,12 @@
         <v>177</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>178</v>
@@ -2086,12 +2028,12 @@
         <v>179</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>180</v>
@@ -2100,12 +2042,12 @@
         <v>181</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>182</v>
@@ -2114,12 +2056,12 @@
         <v>183</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>184</v>
@@ -2128,12 +2070,12 @@
         <v>185</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>186</v>
@@ -2142,12 +2084,12 @@
         <v>8</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>187</v>
@@ -2156,12 +2098,12 @@
         <v>188</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>189</v>
@@ -2170,12 +2112,12 @@
         <v>190</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>412</v>
+        <v>436</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>191</v>
@@ -2184,12 +2126,12 @@
         <v>192</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>194</v>
@@ -2198,12 +2140,12 @@
         <v>195</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>196</v>
@@ -2212,12 +2154,12 @@
         <v>197</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>198</v>
@@ -2226,12 +2168,12 @@
         <v>199</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>200</v>
@@ -2240,12 +2182,12 @@
         <v>201</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>202</v>
@@ -2254,12 +2196,12 @@
         <v>203</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>204</v>
@@ -2268,12 +2210,12 @@
         <v>205</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>206</v>
@@ -2282,12 +2224,12 @@
         <v>207</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>208</v>
@@ -2296,12 +2238,12 @@
         <v>209</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>210</v>
@@ -2310,12 +2252,12 @@
         <v>211</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>212</v>
@@ -2324,7 +2266,7 @@
         <v>213</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
@@ -2338,7 +2280,7 @@
         <v>216</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
@@ -2352,7 +2294,7 @@
         <v>218</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
@@ -2366,7 +2308,7 @@
         <v>220</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
@@ -2380,7 +2322,7 @@
         <v>222</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
@@ -2394,7 +2336,7 @@
         <v>224</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
@@ -2408,7 +2350,7 @@
         <v>226</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
@@ -2422,7 +2364,7 @@
         <v>228</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
@@ -2436,7 +2378,7 @@
         <v>230</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
@@ -2450,7 +2392,7 @@
         <v>232</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
@@ -2464,7 +2406,7 @@
         <v>234</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
@@ -2478,7 +2420,7 @@
         <v>236</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
@@ -2492,7 +2434,7 @@
         <v>238</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
@@ -2506,7 +2448,7 @@
         <v>240</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
@@ -2520,7 +2462,7 @@
         <v>242</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
@@ -2534,7 +2476,7 @@
         <v>244</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
@@ -2548,7 +2490,7 @@
         <v>246</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
@@ -2562,7 +2504,7 @@
         <v>248</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
@@ -2576,7 +2518,7 @@
         <v>250</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
@@ -2590,7 +2532,7 @@
         <v>252</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
@@ -2604,7 +2546,7 @@
         <v>254</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
@@ -2618,7 +2560,7 @@
         <v>258</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
@@ -2632,7 +2574,7 @@
         <v>260</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
@@ -2646,7 +2588,7 @@
         <v>262</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
@@ -2660,7 +2602,7 @@
         <v>264</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
@@ -2674,7 +2616,7 @@
         <v>266</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
@@ -2688,7 +2630,7 @@
         <v>268</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
@@ -2702,7 +2644,7 @@
         <v>270</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
@@ -2716,7 +2658,7 @@
         <v>272</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
@@ -2730,7 +2672,7 @@
         <v>274</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
@@ -2744,7 +2686,7 @@
         <v>276</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
@@ -2758,7 +2700,7 @@
         <v>279</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.4">
@@ -2772,7 +2714,7 @@
         <v>281</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
@@ -2786,7 +2728,7 @@
         <v>283</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
@@ -2800,7 +2742,7 @@
         <v>285</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.4">
@@ -2814,7 +2756,7 @@
         <v>287</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.4">
@@ -2828,7 +2770,7 @@
         <v>289</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.4">
@@ -2842,7 +2784,7 @@
         <v>291</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.4">
@@ -2856,7 +2798,7 @@
         <v>293</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.4">
@@ -2870,7 +2812,7 @@
         <v>295</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.4">
@@ -2884,7 +2826,7 @@
         <v>297</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.4">
@@ -2898,7 +2840,7 @@
         <v>300</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.4">
@@ -2912,7 +2854,7 @@
         <v>302</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.4">
@@ -2926,7 +2868,7 @@
         <v>304</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.4">
@@ -2940,7 +2882,7 @@
         <v>306</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
@@ -2954,7 +2896,7 @@
         <v>308</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.4">
@@ -2968,7 +2910,7 @@
         <v>310</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.4">
@@ -2982,7 +2924,7 @@
         <v>312</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.4">
@@ -2996,7 +2938,7 @@
         <v>314</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.4">
@@ -3010,7 +2952,7 @@
         <v>316</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.4">
@@ -3024,7 +2966,7 @@
         <v>318</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.4">
@@ -3038,7 +2980,7 @@
         <v>321</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.4">
@@ -3052,7 +2994,7 @@
         <v>323</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.4">
@@ -3066,7 +3008,7 @@
         <v>325</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.4">
@@ -3080,7 +3022,7 @@
         <v>327</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.4">
@@ -3094,7 +3036,7 @@
         <v>329</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.4">
@@ -3108,7 +3050,7 @@
         <v>331</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.4">
@@ -3122,7 +3064,7 @@
         <v>333</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.4">
@@ -3136,7 +3078,7 @@
         <v>335</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.4">
@@ -3150,7 +3092,7 @@
         <v>337</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.4">
@@ -3164,7 +3106,7 @@
         <v>339</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.4">
@@ -3178,7 +3120,7 @@
         <v>342</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.4">
@@ -3192,7 +3134,7 @@
         <v>344</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.4">
@@ -3206,7 +3148,7 @@
         <v>346</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.4">
@@ -3220,7 +3162,7 @@
         <v>348</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.4">
@@ -3234,7 +3176,7 @@
         <v>350</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.4">
@@ -3248,7 +3190,7 @@
         <v>352</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.4">
@@ -3262,7 +3204,7 @@
         <v>354</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.4">
@@ -3276,7 +3218,7 @@
         <v>356</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.4">
@@ -3290,7 +3232,7 @@
         <v>358</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.4">
@@ -3304,7 +3246,7 @@
         <v>360</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.4">
@@ -3318,7 +3260,7 @@
         <v>363</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.4">
@@ -3332,7 +3274,7 @@
         <v>365</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.4">
@@ -3346,7 +3288,7 @@
         <v>367</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.4">
@@ -3360,7 +3302,7 @@
         <v>369</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.4">
@@ -3374,7 +3316,7 @@
         <v>371</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.4">
@@ -3388,7 +3330,7 @@
         <v>373</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.4">
@@ -3402,7 +3344,7 @@
         <v>375</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.4">
@@ -3416,7 +3358,7 @@
         <v>377</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.4">
@@ -3430,7 +3372,7 @@
         <v>379</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.4">
@@ -3444,7 +3386,7 @@
         <v>381</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.4">
@@ -3458,7 +3400,7 @@
         <v>384</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.4">
@@ -3472,7 +3414,7 @@
         <v>386</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.4">
@@ -3486,7 +3428,7 @@
         <v>388</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.4">
@@ -3500,7 +3442,7 @@
         <v>390</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.4">
@@ -3514,7 +3456,7 @@
         <v>392</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.4">
@@ -3528,7 +3470,7 @@
         <v>394</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.4">
@@ -3542,7 +3484,7 @@
         <v>396</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.4">
@@ -3556,7 +3498,7 @@
         <v>398</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.4">
@@ -3570,7 +3512,7 @@
         <v>400</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.4">
@@ -3584,7 +3526,7 @@
         <v>402</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.4">
@@ -3592,13 +3534,13 @@
         <v>411</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>403</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.4">
@@ -3606,13 +3548,13 @@
         <v>411</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>404</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.4">
@@ -3620,13 +3562,13 @@
         <v>411</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>405</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.4">
@@ -3634,13 +3576,13 @@
         <v>411</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>406</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.4">
@@ -3648,13 +3590,13 @@
         <v>411</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>407</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.4">
@@ -3662,13 +3604,13 @@
         <v>411</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>408</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.4">
@@ -3676,13 +3618,13 @@
         <v>411</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>409</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.4">
@@ -3690,13 +3632,13 @@
         <v>411</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>410</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -3849,8 +3791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEEDF3A-A049-6040-B82C-825BD7BF40EE}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -4276,7 +4218,7 @@
         <v>96</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -4522,7 +4464,7 @@
         <v>129</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
@@ -4727,7 +4669,7 @@
         <v>159</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
@@ -4768,7 +4710,7 @@
         <v>165</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Finalizing Value chain flow
</commit_message>
<xml_diff>
--- a/client/public/VC_Capability_Master.xlsx
+++ b/client/public/VC_Capability_Master.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Project\ValueChainSite\ValueChainIntelligence\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6309EC1-81DA-4D7C-9001-C119FF0084EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D9F6F1-1ECA-449C-88B8-0D16FF4C9BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BD5DD5E2-53C9-C848-BED8-5645BBCDEF26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{BD5DD5E2-53C9-C848-BED8-5645BBCDEF26}"/>
   </bookViews>
   <sheets>
     <sheet name="Homepage" sheetId="5" r:id="rId1"/>
     <sheet name="Value Chain Master" sheetId="4" r:id="rId2"/>
     <sheet name="Capability Attributes" sheetId="2" r:id="rId3"/>
     <sheet name="Capability Master" sheetId="1" r:id="rId4"/>
+    <sheet name="Maturity Mapping" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Capability Master'!$A$1:$M$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Maturity Mapping'!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="449">
   <si>
     <t>Capability Name</t>
   </si>
@@ -1347,13 +1349,55 @@
   </si>
   <si>
     <t>Shipping, Logistics (3PL/4PL/Forwarders - NVOCC), Retail (General Merchandise)</t>
+  </si>
+  <si>
+    <t>];</t>
+  </si>
+  <si>
+    <t>Technology Maturity Levels</t>
+  </si>
+  <si>
+    <t>Business Maturity Levels</t>
+  </si>
+  <si>
+    <t>Maturity Level</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Manual/Offline</t>
+  </si>
+  <si>
+    <t>Digitized</t>
+  </si>
+  <si>
+    <t>Integrated Systems</t>
+  </si>
+  <si>
+    <t>Smart / Connected</t>
+  </si>
+  <si>
+    <t>Intelligent / Predictive</t>
+  </si>
+  <si>
+    <t>Ad hoc</t>
+  </si>
+  <si>
+    <t>Statndardized</t>
+  </si>
+  <si>
+    <t>Integrated</t>
+  </si>
+  <si>
+    <t>Leading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1416,6 +1460,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFC586C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1458,7 +1520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1475,6 +1537,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1814,7 +1885,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -4724,4 +4795,328 @@
   <autoFilter ref="A1:M23" xr:uid="{6AEEDF3A-A049-6040-B82C-825BD7BF40EE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DDD45B-FE83-47AE-9E68-616AB411BDE9}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>448</v>
+      </c>
+      <c r="B6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>445</v>
+      </c>
+      <c r="B7" t="s">
+        <v>441</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>446</v>
+      </c>
+      <c r="B9" t="s">
+        <v>441</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>447</v>
+      </c>
+      <c r="B10" t="s">
+        <v>441</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>448</v>
+      </c>
+      <c r="B11" t="s">
+        <v>441</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>445</v>
+      </c>
+      <c r="B12" t="s">
+        <v>442</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>439</v>
+      </c>
+      <c r="B13" t="s">
+        <v>442</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>446</v>
+      </c>
+      <c r="B14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>447</v>
+      </c>
+      <c r="B15" t="s">
+        <v>442</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>448</v>
+      </c>
+      <c r="B16" t="s">
+        <v>442</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>445</v>
+      </c>
+      <c r="B17" t="s">
+        <v>443</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>439</v>
+      </c>
+      <c r="B18" t="s">
+        <v>443</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>446</v>
+      </c>
+      <c r="B19" t="s">
+        <v>443</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>447</v>
+      </c>
+      <c r="B20" t="s">
+        <v>443</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>448</v>
+      </c>
+      <c r="B21" t="s">
+        <v>443</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>445</v>
+      </c>
+      <c r="B22" t="s">
+        <v>444</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>439</v>
+      </c>
+      <c r="B23" t="s">
+        <v>444</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B24" t="s">
+        <v>444</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>447</v>
+      </c>
+      <c r="B25" t="s">
+        <v>444</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>448</v>
+      </c>
+      <c r="B26" t="s">
+        <v>444</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C26" xr:uid="{97DDD45B-FE83-47AE-9E68-616AB411BDE9}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Strategy Initiative initial checking
</commit_message>
<xml_diff>
--- a/client/public/VC_Capability_Master.xlsx
+++ b/client/public/VC_Capability_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Project\ValueChainSite\ValueChainIntelligence\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D9F6F1-1ECA-449C-88B8-0D16FF4C9BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C81D840-80DB-472E-B5B9-064D5BF82106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{BD5DD5E2-53C9-C848-BED8-5645BBCDEF26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{BD5DD5E2-53C9-C848-BED8-5645BBCDEF26}"/>
   </bookViews>
   <sheets>
     <sheet name="Homepage" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Capability Attributes" sheetId="2" r:id="rId3"/>
     <sheet name="Capability Master" sheetId="1" r:id="rId4"/>
     <sheet name="Maturity Mapping" sheetId="6" r:id="rId5"/>
+    <sheet name="Buy or Build" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Capability Master'!$A$1:$M$23</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="457">
   <si>
     <t>Capability Name</t>
   </si>
@@ -1391,6 +1392,33 @@
   </si>
   <si>
     <t>Leading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capability Name </t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building this capability does not provide any competitive edge. Hence, recommendation is to buy </t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building this capability provides a competitive edge. Hence, recommendation is to build </t>
+  </si>
+  <si>
+    <t>Buy/Build Description</t>
+  </si>
+  <si>
+    <t>Suggestions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 1
+Example 2
+Build
+</t>
   </si>
 </sst>
 </file>
@@ -1520,7 +1548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1545,6 +1573,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3828,8 +3859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEEDF3A-A049-6040-B82C-825BD7BF40EE}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -4801,7 +4832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DDD45B-FE83-47AE-9E68-616AB411BDE9}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -5119,4 +5150,415 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CB7485-6F0B-48FA-9047-35ECC73755D2}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.08203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="E1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>432</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>432</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>432</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>432</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" t="s">
+        <v>432</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" t="s">
+        <v>432</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>432</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>432</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>432</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" t="s">
+        <v>432</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" t="s">
+        <v>432</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="s">
+        <v>432</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" t="s">
+        <v>432</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="64" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" t="s">
+        <v>432</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>